<commit_message>
- try ejb's with different transaction levels
</commit_message>
<xml_diff>
--- a/ejbrace/Race results.xlsx
+++ b/ejbrace/Race results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
   <si>
     <t>Run 1</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Remote EJB (Default Transaction)</t>
+  </si>
+  <si>
+    <t>Remote EJB (Transaction Never)</t>
+  </si>
+  <si>
+    <t>Remote EJB (Transaction Supports)</t>
   </si>
 </sst>
 </file>
@@ -256,10 +262,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.5302153700007344E-2"/>
+          <c:x val="6.526292091246233E-2"/>
           <c:y val="6.7167576857929651E-2"/>
-          <c:w val="0.84085159535780918"/>
-          <c:h val="0.73773766689759801"/>
+          <c:w val="0.87089086288358375"/>
+          <c:h val="0.77012922374662163"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -702,21 +708,51 @@
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="5"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$41</c:f>
+              <c:f>Sheet1!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Local EJB</c:v>
+                  <c:v>Remote EJB (Transaction Never)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -724,7 +760,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -735,11 +771,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent5"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -786,39 +822,163 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$45:$K$45</c:f>
+              <c:f>Sheet1!$B$53:$K$53</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.214</c:v>
+                  <c:v>54.567999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14199999999999999</c:v>
+                  <c:v>54.924999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>53.372</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10100000000000001</c:v>
+                  <c:v>54.512999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.6999999999999999E-2</c:v>
+                  <c:v>53.609000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>52.802</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2E-2</c:v>
+                  <c:v>53.405000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2999999999999999E-2</c:v>
+                  <c:v>52.424999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0999999999999999E-2</c:v>
+                  <c:v>53.290999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4E-2</c:v>
+                  <c:v>53.039000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remote EJB (Transaction Supports)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$61:$K$61</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>53.058</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.466000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.250999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.173999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.005000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54.345999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52.673999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.655999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.162999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -833,11 +993,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="352677040"/>
-        <c:axId val="352676256"/>
+        <c:axId val="348716632"/>
+        <c:axId val="348715848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="352677040"/>
+        <c:axId val="348716632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,14 +1054,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352676256"/>
+        <c:crossAx val="348715848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352676256"/>
+        <c:axId val="348715848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -956,7 +1117,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352677040"/>
+        <c:crossAx val="348716632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,16 +1758,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>557645</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>404814</xdr:colOff>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>59228</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>83127</xdr:rowOff>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1891,14 +2052,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A9" sqref="A9"/>
       <selection pane="topRight" activeCell="B9" sqref="B9"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11:K15"/>
+      <selection pane="bottomRight" activeCell="K59" sqref="K59:K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2929,19 +3090,39 @@
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6" t="e">
+      <c r="B37" s="6">
+        <v>35</v>
+      </c>
+      <c r="C37" s="6">
+        <v>35</v>
+      </c>
+      <c r="D37" s="6">
+        <v>35</v>
+      </c>
+      <c r="E37" s="6">
+        <v>35</v>
+      </c>
+      <c r="F37" s="6">
+        <v>35</v>
+      </c>
+      <c r="G37" s="6">
+        <v>35</v>
+      </c>
+      <c r="H37" s="6">
+        <v>35</v>
+      </c>
+      <c r="I37" s="6">
+        <v>35</v>
+      </c>
+      <c r="J37" s="6">
+        <v>35</v>
+      </c>
+      <c r="K37" s="6">
+        <v>35</v>
+      </c>
+      <c r="L37" s="6">
         <f xml:space="preserve"> SUM(B37:K37) / COUNT(B37:K37)</f>
-        <v>#DIV/0!</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -3229,8 +3410,504 @@
         <v>5.7</v>
       </c>
     </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="4">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>3</v>
+      </c>
+      <c r="E50" s="4">
+        <v>4</v>
+      </c>
+      <c r="F50" s="4">
+        <v>5</v>
+      </c>
+      <c r="G50" s="4">
+        <v>6</v>
+      </c>
+      <c r="H50" s="4">
+        <v>7</v>
+      </c>
+      <c r="I50" s="4">
+        <v>8</v>
+      </c>
+      <c r="J50" s="4">
+        <v>9</v>
+      </c>
+      <c r="K50" s="4">
+        <v>10</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="C51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="G51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="H51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="I51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="J51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="K51" s="6">
+        <v>2000</v>
+      </c>
+      <c r="L51" s="6">
+        <f xml:space="preserve"> SUM(B51:K51) / COUNT(B51:K51)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="6">
+        <v>109135</v>
+      </c>
+      <c r="C52" s="6">
+        <v>109849</v>
+      </c>
+      <c r="D52" s="6">
+        <v>106744</v>
+      </c>
+      <c r="E52" s="6">
+        <v>109025</v>
+      </c>
+      <c r="F52" s="6">
+        <v>107217</v>
+      </c>
+      <c r="G52" s="6">
+        <v>105604</v>
+      </c>
+      <c r="H52" s="6">
+        <v>106809</v>
+      </c>
+      <c r="I52" s="6">
+        <v>104850</v>
+      </c>
+      <c r="J52" s="6">
+        <v>106582</v>
+      </c>
+      <c r="K52" s="6">
+        <v>106078</v>
+      </c>
+      <c r="L52" s="6">
+        <f xml:space="preserve"> SUM(B52:K52) / COUNT(B52:K52)</f>
+        <v>107189.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="6">
+        <v>54.567999999999998</v>
+      </c>
+      <c r="C53" s="6">
+        <v>54.924999999999997</v>
+      </c>
+      <c r="D53" s="6">
+        <v>53.372</v>
+      </c>
+      <c r="E53" s="6">
+        <v>54.512999999999998</v>
+      </c>
+      <c r="F53" s="6">
+        <v>53.609000000000002</v>
+      </c>
+      <c r="G53" s="6">
+        <v>52.802</v>
+      </c>
+      <c r="H53" s="6">
+        <v>53.405000000000001</v>
+      </c>
+      <c r="I53" s="6">
+        <v>52.424999999999997</v>
+      </c>
+      <c r="J53" s="6">
+        <v>53.290999999999997</v>
+      </c>
+      <c r="K53" s="6">
+        <v>53.039000000000001</v>
+      </c>
+      <c r="L53" s="6">
+        <f xml:space="preserve"> SUM(B53:K53) / COUNT(B53:K53)</f>
+        <v>53.59490000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="6">
+        <v>40</v>
+      </c>
+      <c r="C54" s="6">
+        <v>41</v>
+      </c>
+      <c r="D54" s="6">
+        <v>41</v>
+      </c>
+      <c r="E54" s="6">
+        <v>40</v>
+      </c>
+      <c r="F54" s="6">
+        <v>39</v>
+      </c>
+      <c r="G54" s="6">
+        <v>39</v>
+      </c>
+      <c r="H54" s="6">
+        <v>39</v>
+      </c>
+      <c r="I54" s="6">
+        <v>40</v>
+      </c>
+      <c r="J54" s="6">
+        <v>41</v>
+      </c>
+      <c r="K54" s="6">
+        <v>39</v>
+      </c>
+      <c r="L54" s="6">
+        <f xml:space="preserve"> SUM(B54:K54) / COUNT(B54:K54)</f>
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="6">
+        <v>102</v>
+      </c>
+      <c r="C55" s="6">
+        <v>128</v>
+      </c>
+      <c r="D55" s="6">
+        <v>211</v>
+      </c>
+      <c r="E55" s="6">
+        <v>1113</v>
+      </c>
+      <c r="F55" s="6">
+        <v>422</v>
+      </c>
+      <c r="G55" s="6">
+        <v>118</v>
+      </c>
+      <c r="H55" s="6">
+        <v>378</v>
+      </c>
+      <c r="I55" s="6">
+        <v>112</v>
+      </c>
+      <c r="J55" s="6">
+        <v>170</v>
+      </c>
+      <c r="K55" s="6">
+        <v>118</v>
+      </c>
+      <c r="L55" s="6">
+        <f xml:space="preserve"> SUM(B55:K55) / COUNT(B55:K55)</f>
+        <v>287.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4">
+        <v>1</v>
+      </c>
+      <c r="C58" s="4">
+        <v>2</v>
+      </c>
+      <c r="D58" s="4">
+        <v>3</v>
+      </c>
+      <c r="E58" s="4">
+        <v>4</v>
+      </c>
+      <c r="F58" s="4">
+        <v>5</v>
+      </c>
+      <c r="G58" s="4">
+        <v>6</v>
+      </c>
+      <c r="H58" s="4">
+        <v>7</v>
+      </c>
+      <c r="I58" s="4">
+        <v>8</v>
+      </c>
+      <c r="J58" s="4">
+        <v>9</v>
+      </c>
+      <c r="K58" s="4">
+        <v>10</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="C59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="G59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="H59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="I59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="J59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="K59" s="6">
+        <v>2000</v>
+      </c>
+      <c r="L59" s="6">
+        <f xml:space="preserve"> SUM(B59:K59) / COUNT(B59:K59)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="6">
+        <v>106115</v>
+      </c>
+      <c r="C60" s="6">
+        <v>105395</v>
+      </c>
+      <c r="D60" s="6">
+        <v>106931</v>
+      </c>
+      <c r="E60" s="6">
+        <v>106501</v>
+      </c>
+      <c r="F60" s="6">
+        <v>108347</v>
+      </c>
+      <c r="G60" s="6">
+        <v>108010</v>
+      </c>
+      <c r="H60" s="6">
+        <v>108691</v>
+      </c>
+      <c r="I60" s="6">
+        <v>105347</v>
+      </c>
+      <c r="J60" s="6">
+        <v>107312</v>
+      </c>
+      <c r="K60" s="6">
+        <v>110325</v>
+      </c>
+      <c r="L60" s="6">
+        <f xml:space="preserve"> SUM(B60:K60) / COUNT(B60:K60)</f>
+        <v>107297.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="6">
+        <v>53.058</v>
+      </c>
+      <c r="C61" s="6">
+        <v>52.698</v>
+      </c>
+      <c r="D61" s="6">
+        <v>53.466000000000001</v>
+      </c>
+      <c r="E61" s="6">
+        <v>53.250999999999998</v>
+      </c>
+      <c r="F61" s="6">
+        <v>54.173999999999999</v>
+      </c>
+      <c r="G61" s="6">
+        <v>54.005000000000003</v>
+      </c>
+      <c r="H61" s="6">
+        <v>54.345999999999997</v>
+      </c>
+      <c r="I61" s="6">
+        <v>52.673999999999999</v>
+      </c>
+      <c r="J61" s="6">
+        <v>53.655999999999999</v>
+      </c>
+      <c r="K61" s="6">
+        <v>55.162999999999997</v>
+      </c>
+      <c r="L61" s="6">
+        <f xml:space="preserve"> SUM(B61:K61) / COUNT(B61:K61)</f>
+        <v>53.649099999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="6">
+        <v>39</v>
+      </c>
+      <c r="C62" s="6">
+        <v>40</v>
+      </c>
+      <c r="D62" s="6">
+        <v>41</v>
+      </c>
+      <c r="E62" s="6">
+        <v>41</v>
+      </c>
+      <c r="F62" s="6">
+        <v>40</v>
+      </c>
+      <c r="G62" s="6">
+        <v>41</v>
+      </c>
+      <c r="H62" s="6">
+        <v>40</v>
+      </c>
+      <c r="I62" s="6">
+        <v>39</v>
+      </c>
+      <c r="J62" s="6">
+        <v>39</v>
+      </c>
+      <c r="K62" s="6">
+        <v>40</v>
+      </c>
+      <c r="L62" s="6">
+        <f xml:space="preserve"> SUM(B62:K62) / COUNT(B62:K62)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="6">
+        <v>384</v>
+      </c>
+      <c r="C63" s="6">
+        <v>113</v>
+      </c>
+      <c r="D63" s="6">
+        <v>185</v>
+      </c>
+      <c r="E63" s="6">
+        <v>106</v>
+      </c>
+      <c r="F63" s="6">
+        <v>114</v>
+      </c>
+      <c r="G63" s="6">
+        <v>96</v>
+      </c>
+      <c r="H63" s="6">
+        <v>427</v>
+      </c>
+      <c r="I63" s="6">
+        <v>110</v>
+      </c>
+      <c r="J63" s="6">
+        <v>109</v>
+      </c>
+      <c r="K63" s="6">
+        <v>169</v>
+      </c>
+      <c r="L63" s="6">
+        <f xml:space="preserve"> SUM(B63:K63) / COUNT(B63:K63)</f>
+        <v>181.3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A57:C57"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A25:C25"/>

</xml_diff>